<commit_message>
Removed planegeometry from the index
</commit_message>
<xml_diff>
--- a/CG - Homework 1 - WebGL Neighborhood - Evaluation form.xlsx
+++ b/CG - Homework 1 - WebGL Neighborhood - Evaluation form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\kill-your-neighbourhood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE9D267-E5B7-4DF2-BD94-08270A3D8AE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908495D1-40E6-456A-AAF4-1FF98759BE3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23196" yWindow="5268" windowWidth="23352" windowHeight="12672" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-68" yWindow="-68" windowWidth="28936" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation form" sheetId="1" r:id="rId1"/>
@@ -162,9 +162,6 @@
     <t>Puja Buter-Fadte</t>
   </si>
   <si>
-    <t>We created a neighborhood where two cars pass by, one playing a song from their radio. Behind you is a forest, where an UFO has stolen a car that's moving up and down.</t>
-  </si>
-  <si>
     <t>We make use of color, mapping, refractionRatio, side, opacity and transparent.</t>
   </si>
   <si>
@@ -199,6 +196,22 @@
   </si>
   <si>
     <t>S1129557</t>
+  </si>
+  <si>
+    <r>
+      <t>We created a neighborhood where two cars pass by, one playing a song from their radio. Behind you is a forest, where an UFO has stolen a car that's moving up and down.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> IMPORTANT: The UFO is only visible in firefox (make sure that in the about:config the privacy.file_unique_origin is on false!), due a bug with the loading of the textures. This is not something we can fix, which is why we have made a video that you can find in this project.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1050,8 +1063,8 @@
   </sheetPr>
   <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1099,7 +1112,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="20"/>
     </row>
@@ -1108,7 +1121,7 @@
         <v>28</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="31"/>
     </row>
@@ -1182,7 +1195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:10" ht="141.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1192,7 +1205,7 @@
       </c>
       <c r="F17" s="22"/>
       <c r="H17" s="23" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.45">
@@ -1218,7 +1231,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="8"/>
       <c r="H20" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="57" x14ac:dyDescent="0.45">
@@ -1228,7 +1241,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="9"/>
       <c r="H21" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.45">
@@ -1238,7 +1251,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="9"/>
       <c r="H22" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
@@ -1248,7 +1261,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="9"/>
       <c r="H23" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
@@ -1258,7 +1271,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="9"/>
       <c r="H24" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.45">
@@ -1278,7 +1291,7 @@
       <c r="E26" s="5"/>
       <c r="F26" s="9"/>
       <c r="H26" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
@@ -1288,7 +1301,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="10"/>
       <c r="H27" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1331,7 +1344,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="8"/>
       <c r="H32" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J32" s="15" t="s">
         <v>21</v>
@@ -1344,7 +1357,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="25"/>
       <c r="H33" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J33" s="27"/>
     </row>
@@ -1355,7 +1368,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="10"/>
       <c r="H34" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J34" s="16" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Update CG - Homework 1 - WebGL Neighborhood - Evaluation form.xlsx
</commit_message>
<xml_diff>
--- a/CG - Homework 1 - WebGL Neighborhood - Evaluation form.xlsx
+++ b/CG - Homework 1 - WebGL Neighborhood - Evaluation form.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\kill-your-neighbourhood\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\kill-your-neighbourhood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908495D1-40E6-456A-AAF4-1FF98759BE3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE8D8BF-2BA8-4195-91FA-F0F75B0CA3C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68" yWindow="-68" windowWidth="28936" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation form" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> IMPORTANT: The UFO is only visible in firefox (make sure that in the about:config the privacy.file_unique_origin is on false!), due a bug with the loading of the textures. This is not something we can fix, which is why we have made a video that you can find in this project.</t>
+      <t xml:space="preserve"> IMPORTANT: The UFO is only visible in firefox (make sure that in the about:config the privacy.file_unique_origin is on false!), due a bug with the loading of the textures. This is not something we can fix, which is why we have supplied a video that can be found in this project.</t>
     </r>
   </si>
 </sst>
@@ -715,7 +715,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -738,7 +738,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1063,31 +1063,31 @@
   </sheetPr>
   <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="2.73046875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.73046875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.73046875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.73046875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="40.73046875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2.73046875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="40.73046875" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="2" width="2.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="40.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="40.77734375" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="F4" s="33"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="F6" s="20"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="F7" s="31"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="F8" s="31"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="F9" s="31"/>
     </row>
-    <row r="10" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="F10" s="35"/>
     </row>
-    <row r="12" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1163,25 +1163,25 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="141.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:10" ht="141.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1208,11 +1208,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="1" t="s">
         <v>23</v>
       </c>
@@ -1304,11 +1304,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E28" s="11"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1318,11 +1318,11 @@
       </c>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E30" s="11"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
         <v>15</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:10" ht="72" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>19</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
         <v>37</v>
       </c>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="J33" s="27"/>
     </row>
-    <row r="34" spans="2:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C34" s="1" t="s">
         <v>34</v>
       </c>
@@ -1374,11 +1374,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E35" s="11"/>
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
@@ -1402,32 +1402,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0c2036bf52fce6a572da55f07fac53b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46a6dac1cb1c034944cf78d34111dc32" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1667,10 +1641,48 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AE383F4-3C5F-4177-A300-408FED8DDE00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1694,21 +1706,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AE383F4-3C5F-4177-A300-408FED8DDE00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated the evaluation form
</commit_message>
<xml_diff>
--- a/CG - Homework 1 - WebGL Neighborhood - Evaluation form.xlsx
+++ b/CG - Homework 1 - WebGL Neighborhood - Evaluation form.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\kill-your-neighbourhood\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\kill-your-neighbourhood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C1AFE5-34DA-4655-9FAD-5533F39B08C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24957413-FA67-4182-8146-9AFEEF49F6C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation form" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>We make use of color, mapping, refractionRatio, side, opacity and transparent.</t>
   </si>
   <si>
-    <t>You can use WS to move forward/backward, AD to move left/right and QE to move up/down.</t>
-  </si>
-  <si>
     <t>Houses, trees, lampposts, clock, floors, cars and an ufo.</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
       </rPr>
       <t xml:space="preserve"> IMPORTANT: The UFO is only visible in firefox (make sure that in the about:config the privacy.file_unique_origin is on false!), due a bug with the loading of the textures. This is not something we can fix, that is why we have supplied a video that shows the UFO.</t>
     </r>
+  </si>
+  <si>
+    <t>You can use WS to move forward/backward, AD to move left/right and QE to move up/down. We use the PointerLockControls for this.</t>
   </si>
 </sst>
 </file>
@@ -715,7 +715,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -738,7 +738,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1063,31 +1063,31 @@
   </sheetPr>
   <dimension ref="B2:J36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="2.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="35.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="40.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="40.77734375" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" width="2.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="40.796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="40.796875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.45">
       <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="F4" s="33"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1107,25 +1107,25 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="20"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="31"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="F8" s="31"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="F9" s="31"/>
     </row>
-    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="F10" s="35"/>
     </row>
-    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1163,25 +1163,25 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="141.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="141.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1205,14 +1205,14 @@
       </c>
       <c r="F17" s="22"/>
       <c r="H17" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1224,37 +1224,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="8"/>
       <c r="H20" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="57" x14ac:dyDescent="0.45">
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="9"/>
       <c r="H21" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="9"/>
       <c r="H22" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1264,17 +1264,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="C24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="9"/>
       <c r="H24" s="17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
@@ -1284,31 +1284,31 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="9"/>
       <c r="H26" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="10"/>
       <c r="H27" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E28" s="11"/>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1318,11 +1318,11 @@
       </c>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E30" s="11"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B31" s="2" t="s">
         <v>15</v>
       </c>
@@ -1337,48 +1337,48 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" ht="71.25" x14ac:dyDescent="0.45">
       <c r="C32" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="8"/>
       <c r="H32" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J32" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
       <c r="C33" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="25"/>
       <c r="H33" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J33" s="27"/>
     </row>
-    <row r="34" spans="2:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:10" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C34" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="10"/>
       <c r="H34" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J34" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E35" s="11"/>
       <c r="F35" s="12"/>
     </row>
-    <row r="36" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
@@ -1402,32 +1402,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0c2036bf52fce6a572da55f07fac53b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46a6dac1cb1c034944cf78d34111dc32" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1667,10 +1641,48 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AE383F4-3C5F-4177-A300-408FED8DDE00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1694,21 +1706,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AE383F4-3C5F-4177-A300-408FED8DDE00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>